<commit_message>
Jun 17, 2024, 9:29 PM
</commit_message>
<xml_diff>
--- a/Main/static/CSVs/Features List.xlsx
+++ b/Main/static/CSVs/Features List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitProjects\CS50-FinalProject\Main\static\CSVs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BABC9DC-3941-40D8-BC9A-D58386A3CA69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20CCA78C-346B-44CF-A5CE-B0962AD7DEF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pc_features_text" sheetId="3" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2855" uniqueCount="888">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2975" uniqueCount="888">
   <si>
     <t>Metadata:</t>
   </si>
@@ -3090,8 +3090,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1000DAD0-45D8-4F57-BB32-ED68B84F1CCC}">
   <dimension ref="A1:F910"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F1" sqref="A1:F1"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B908" sqref="B2:B908"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21317,8 +21317,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF617F07-646C-48AF-866C-AB0475963108}">
   <dimension ref="B1:N307"/>
   <sheetViews>
-    <sheetView topLeftCell="A231" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:L268"/>
+    <sheetView topLeftCell="A280" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:L307"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26706,7 +26706,7 @@
         <v>541</v>
       </c>
       <c r="C178">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D178">
         <v>8</v>
@@ -26735,7 +26735,7 @@
         <v>543</v>
       </c>
       <c r="C179">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D179">
         <v>8</v>
@@ -26764,7 +26764,7 @@
         <v>534</v>
       </c>
       <c r="C180">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="D180">
         <v>8</v>
@@ -26793,7 +26793,7 @@
         <v>536</v>
       </c>
       <c r="C181">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D181">
         <v>8</v>
@@ -26822,7 +26822,7 @@
         <v>539</v>
       </c>
       <c r="C182">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D182">
         <v>8</v>
@@ -29365,6 +29365,15 @@
       </c>
     </row>
     <row r="269" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B269">
+        <v>791</v>
+      </c>
+      <c r="C269">
+        <v>267</v>
+      </c>
+      <c r="D269">
+        <v>11</v>
+      </c>
       <c r="F269" t="s">
         <v>883</v>
       </c>
@@ -29383,7 +29392,7 @@
         <v>794</v>
       </c>
       <c r="C270">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D270">
         <v>11</v>
@@ -29412,7 +29421,7 @@
         <v>797</v>
       </c>
       <c r="C271">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="D271">
         <v>11</v>
@@ -29441,7 +29450,7 @@
         <v>799</v>
       </c>
       <c r="C272">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D272">
         <v>11</v>
@@ -29470,7 +29479,7 @@
         <v>802</v>
       </c>
       <c r="C273">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D273">
         <v>11</v>
@@ -29499,7 +29508,7 @@
         <v>805</v>
       </c>
       <c r="C274">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D274">
         <v>11</v>
@@ -29528,7 +29537,7 @@
         <v>808</v>
       </c>
       <c r="C275">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D275">
         <v>11</v>
@@ -29557,7 +29566,7 @@
         <v>811</v>
       </c>
       <c r="C276">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D276">
         <v>11</v>
@@ -29586,7 +29595,7 @@
         <v>814</v>
       </c>
       <c r="C277">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="D277">
         <v>11</v>
@@ -29615,7 +29624,7 @@
         <v>816</v>
       </c>
       <c r="C278">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D278">
         <v>11</v>
@@ -29644,7 +29653,7 @@
         <v>819</v>
       </c>
       <c r="C279">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="D279">
         <v>11</v>
@@ -29673,7 +29682,7 @@
         <v>822</v>
       </c>
       <c r="C280">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D280">
         <v>11</v>
@@ -29702,7 +29711,7 @@
         <v>825</v>
       </c>
       <c r="C281">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="D281">
         <v>11</v>
@@ -29731,7 +29740,7 @@
         <v>828</v>
       </c>
       <c r="C282">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="D282">
         <v>11</v>
@@ -29760,7 +29769,7 @@
         <v>831</v>
       </c>
       <c r="C283">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="D283">
         <v>11</v>
@@ -29792,7 +29801,7 @@
         <v>833</v>
       </c>
       <c r="C284">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D284">
         <v>11</v>
@@ -29821,7 +29830,7 @@
         <v>842</v>
       </c>
       <c r="C285">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D285">
         <v>11</v>
@@ -29850,7 +29859,7 @@
         <v>844</v>
       </c>
       <c r="C286">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="D286">
         <v>11</v>
@@ -29879,7 +29888,7 @@
         <v>847</v>
       </c>
       <c r="C287">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D287">
         <v>11</v>
@@ -29908,7 +29917,7 @@
         <v>849</v>
       </c>
       <c r="C288">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D288">
         <v>11</v>
@@ -29937,7 +29946,7 @@
         <v>853</v>
       </c>
       <c r="C289">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="D289">
         <v>12</v>
@@ -29960,7 +29969,7 @@
         <v>855</v>
       </c>
       <c r="C290">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="D290">
         <v>12</v>
@@ -29989,7 +29998,7 @@
         <v>857</v>
       </c>
       <c r="C291">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="D291">
         <v>12</v>
@@ -30018,7 +30027,7 @@
         <v>867</v>
       </c>
       <c r="C292">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D292">
         <v>12</v>
@@ -30047,7 +30056,7 @@
         <v>872</v>
       </c>
       <c r="C293">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D293">
         <v>12</v>
@@ -30076,7 +30085,7 @@
         <v>876</v>
       </c>
       <c r="C294">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="D294">
         <v>12</v>
@@ -30105,7 +30114,7 @@
         <v>878</v>
       </c>
       <c r="C295">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D295">
         <v>12</v>
@@ -30134,7 +30143,7 @@
         <v>880</v>
       </c>
       <c r="C296">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="D296">
         <v>12</v>
@@ -30163,7 +30172,7 @@
         <v>882</v>
       </c>
       <c r="C297">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="D297">
         <v>12</v>
@@ -30192,7 +30201,7 @@
         <v>885</v>
       </c>
       <c r="C298">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D298">
         <v>12</v>
@@ -30224,7 +30233,7 @@
         <v>888</v>
       </c>
       <c r="C299">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="D299">
         <v>12</v>
@@ -30256,7 +30265,7 @@
         <v>890</v>
       </c>
       <c r="C300">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D300">
         <v>12</v>
@@ -30281,6 +30290,12 @@
       </c>
     </row>
     <row r="301" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B301">
+        <v>893</v>
+      </c>
+      <c r="C301">
+        <v>299</v>
+      </c>
       <c r="F301" t="s">
         <v>849</v>
       </c>
@@ -30299,7 +30314,7 @@
         <v>895</v>
       </c>
       <c r="C302">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="D302">
         <v>12</v>
@@ -30328,7 +30343,7 @@
         <v>897</v>
       </c>
       <c r="C303">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="D303">
         <v>12</v>
@@ -30357,7 +30372,7 @@
         <v>899</v>
       </c>
       <c r="C304">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="D304">
         <v>12</v>
@@ -30386,7 +30401,7 @@
         <v>901</v>
       </c>
       <c r="C305">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="D305">
         <v>12</v>
@@ -30415,7 +30430,7 @@
         <v>903</v>
       </c>
       <c r="C306">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="D306">
         <v>12</v>
@@ -30444,7 +30459,7 @@
         <v>905</v>
       </c>
       <c r="C307">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="D307">
         <v>12</v>
@@ -30478,17 +30493,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE29A042-3862-47FE-83B9-65F533A211F7}">
-  <dimension ref="A1:K268"/>
+  <dimension ref="A1:K307"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -35760,7 +35771,7 @@
         <v>541</v>
       </c>
       <c r="B178">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C178">
         <v>8</v>
@@ -35789,7 +35800,7 @@
         <v>543</v>
       </c>
       <c r="B179">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C179">
         <v>8</v>
@@ -35818,7 +35829,7 @@
         <v>534</v>
       </c>
       <c r="B180">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C180">
         <v>8</v>
@@ -35847,7 +35858,7 @@
         <v>536</v>
       </c>
       <c r="B181">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C181">
         <v>8</v>
@@ -35876,7 +35887,7 @@
         <v>539</v>
       </c>
       <c r="B182">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C182">
         <v>8</v>
@@ -38413,6 +38424,1125 @@
       </c>
       <c r="J268" t="s">
         <v>720</v>
+      </c>
+    </row>
+    <row r="269" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A269">
+        <v>791</v>
+      </c>
+      <c r="B269">
+        <v>267</v>
+      </c>
+      <c r="C269">
+        <v>11</v>
+      </c>
+      <c r="E269" t="s">
+        <v>883</v>
+      </c>
+      <c r="F269" t="s">
+        <v>866</v>
+      </c>
+      <c r="G269">
+        <v>9</v>
+      </c>
+      <c r="J269" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="270" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A270">
+        <v>794</v>
+      </c>
+      <c r="B270">
+        <v>268</v>
+      </c>
+      <c r="C270">
+        <v>11</v>
+      </c>
+      <c r="D270">
+        <v>2</v>
+      </c>
+      <c r="E270" t="s">
+        <v>883</v>
+      </c>
+      <c r="F270" t="s">
+        <v>866</v>
+      </c>
+      <c r="G270">
+        <v>1</v>
+      </c>
+      <c r="I270">
+        <v>0</v>
+      </c>
+      <c r="J270" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="271" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A271">
+        <v>797</v>
+      </c>
+      <c r="B271">
+        <v>269</v>
+      </c>
+      <c r="C271">
+        <v>11</v>
+      </c>
+      <c r="D271">
+        <v>2</v>
+      </c>
+      <c r="E271" t="s">
+        <v>883</v>
+      </c>
+      <c r="F271" t="s">
+        <v>866</v>
+      </c>
+      <c r="G271">
+        <v>1</v>
+      </c>
+      <c r="I271">
+        <v>0</v>
+      </c>
+      <c r="J271" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="272" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A272">
+        <v>799</v>
+      </c>
+      <c r="B272">
+        <v>270</v>
+      </c>
+      <c r="C272">
+        <v>11</v>
+      </c>
+      <c r="D272">
+        <v>2</v>
+      </c>
+      <c r="E272" t="s">
+        <v>883</v>
+      </c>
+      <c r="F272" t="s">
+        <v>866</v>
+      </c>
+      <c r="G272">
+        <v>5</v>
+      </c>
+      <c r="I272">
+        <v>0</v>
+      </c>
+      <c r="J272" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="273" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A273">
+        <v>802</v>
+      </c>
+      <c r="B273">
+        <v>271</v>
+      </c>
+      <c r="C273">
+        <v>11</v>
+      </c>
+      <c r="D273">
+        <v>2</v>
+      </c>
+      <c r="E273" t="s">
+        <v>883</v>
+      </c>
+      <c r="F273" t="s">
+        <v>866</v>
+      </c>
+      <c r="G273">
+        <v>9</v>
+      </c>
+      <c r="I273">
+        <v>0</v>
+      </c>
+      <c r="J273" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="274" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A274">
+        <v>805</v>
+      </c>
+      <c r="B274">
+        <v>272</v>
+      </c>
+      <c r="C274">
+        <v>11</v>
+      </c>
+      <c r="D274">
+        <v>2</v>
+      </c>
+      <c r="E274" t="s">
+        <v>883</v>
+      </c>
+      <c r="F274" t="s">
+        <v>866</v>
+      </c>
+      <c r="G274">
+        <v>1</v>
+      </c>
+      <c r="I274">
+        <v>0</v>
+      </c>
+      <c r="J274" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="275" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A275">
+        <v>808</v>
+      </c>
+      <c r="B275">
+        <v>273</v>
+      </c>
+      <c r="C275">
+        <v>11</v>
+      </c>
+      <c r="D275">
+        <v>2</v>
+      </c>
+      <c r="E275" t="s">
+        <v>883</v>
+      </c>
+      <c r="F275" t="s">
+        <v>866</v>
+      </c>
+      <c r="G275">
+        <v>7</v>
+      </c>
+      <c r="I275">
+        <v>0</v>
+      </c>
+      <c r="J275" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="276" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A276">
+        <v>811</v>
+      </c>
+      <c r="B276">
+        <v>274</v>
+      </c>
+      <c r="C276">
+        <v>11</v>
+      </c>
+      <c r="D276">
+        <v>2</v>
+      </c>
+      <c r="E276" t="s">
+        <v>883</v>
+      </c>
+      <c r="F276" t="s">
+        <v>866</v>
+      </c>
+      <c r="G276">
+        <v>5</v>
+      </c>
+      <c r="I276">
+        <v>0</v>
+      </c>
+      <c r="J276" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="277" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A277">
+        <v>814</v>
+      </c>
+      <c r="B277">
+        <v>275</v>
+      </c>
+      <c r="C277">
+        <v>11</v>
+      </c>
+      <c r="D277">
+        <v>2</v>
+      </c>
+      <c r="E277" t="s">
+        <v>883</v>
+      </c>
+      <c r="F277" t="s">
+        <v>866</v>
+      </c>
+      <c r="G277">
+        <v>1</v>
+      </c>
+      <c r="I277">
+        <v>0</v>
+      </c>
+      <c r="J277" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="278" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A278">
+        <v>816</v>
+      </c>
+      <c r="B278">
+        <v>276</v>
+      </c>
+      <c r="C278">
+        <v>11</v>
+      </c>
+      <c r="D278">
+        <v>2</v>
+      </c>
+      <c r="E278" t="s">
+        <v>883</v>
+      </c>
+      <c r="F278" t="s">
+        <v>866</v>
+      </c>
+      <c r="G278">
+        <v>5</v>
+      </c>
+      <c r="I278">
+        <v>0</v>
+      </c>
+      <c r="J278" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="279" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A279">
+        <v>819</v>
+      </c>
+      <c r="B279">
+        <v>277</v>
+      </c>
+      <c r="C279">
+        <v>11</v>
+      </c>
+      <c r="D279">
+        <v>2</v>
+      </c>
+      <c r="E279" t="s">
+        <v>883</v>
+      </c>
+      <c r="F279" t="s">
+        <v>866</v>
+      </c>
+      <c r="G279">
+        <v>15</v>
+      </c>
+      <c r="I279">
+        <v>0</v>
+      </c>
+      <c r="J279" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="280" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A280">
+        <v>822</v>
+      </c>
+      <c r="B280">
+        <v>278</v>
+      </c>
+      <c r="C280">
+        <v>11</v>
+      </c>
+      <c r="D280">
+        <v>2</v>
+      </c>
+      <c r="E280" t="s">
+        <v>883</v>
+      </c>
+      <c r="F280" t="s">
+        <v>866</v>
+      </c>
+      <c r="G280">
+        <v>3</v>
+      </c>
+      <c r="I280">
+        <v>0</v>
+      </c>
+      <c r="J280" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="281" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A281">
+        <v>825</v>
+      </c>
+      <c r="B281">
+        <v>279</v>
+      </c>
+      <c r="C281">
+        <v>11</v>
+      </c>
+      <c r="D281">
+        <v>2</v>
+      </c>
+      <c r="E281" t="s">
+        <v>883</v>
+      </c>
+      <c r="F281" t="s">
+        <v>866</v>
+      </c>
+      <c r="G281">
+        <v>9</v>
+      </c>
+      <c r="I281">
+        <v>0</v>
+      </c>
+      <c r="J281" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="282" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A282">
+        <v>828</v>
+      </c>
+      <c r="B282">
+        <v>280</v>
+      </c>
+      <c r="C282">
+        <v>11</v>
+      </c>
+      <c r="D282">
+        <v>2</v>
+      </c>
+      <c r="E282" t="s">
+        <v>883</v>
+      </c>
+      <c r="F282" t="s">
+        <v>866</v>
+      </c>
+      <c r="G282">
+        <v>15</v>
+      </c>
+      <c r="I282">
+        <v>0</v>
+      </c>
+      <c r="J282" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="283" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A283">
+        <v>831</v>
+      </c>
+      <c r="B283">
+        <v>281</v>
+      </c>
+      <c r="C283">
+        <v>11</v>
+      </c>
+      <c r="D283">
+        <v>1</v>
+      </c>
+      <c r="E283" t="s">
+        <v>885</v>
+      </c>
+      <c r="F283" t="s">
+        <v>865</v>
+      </c>
+      <c r="G283">
+        <v>1</v>
+      </c>
+      <c r="I283">
+        <v>0</v>
+      </c>
+      <c r="J283" t="s">
+        <v>754</v>
+      </c>
+      <c r="K283" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="284" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A284">
+        <v>833</v>
+      </c>
+      <c r="B284">
+        <v>282</v>
+      </c>
+      <c r="C284">
+        <v>11</v>
+      </c>
+      <c r="D284">
+        <v>2</v>
+      </c>
+      <c r="E284" t="s">
+        <v>885</v>
+      </c>
+      <c r="F284" t="s">
+        <v>865</v>
+      </c>
+      <c r="I284">
+        <v>0</v>
+      </c>
+      <c r="J284" t="s">
+        <v>756</v>
+      </c>
+      <c r="K284" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="285" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A285">
+        <v>842</v>
+      </c>
+      <c r="B285">
+        <v>283</v>
+      </c>
+      <c r="C285">
+        <v>11</v>
+      </c>
+      <c r="D285">
+        <v>2</v>
+      </c>
+      <c r="E285" t="s">
+        <v>885</v>
+      </c>
+      <c r="F285" t="s">
+        <v>865</v>
+      </c>
+      <c r="G285">
+        <v>1</v>
+      </c>
+      <c r="I285">
+        <v>0</v>
+      </c>
+      <c r="J285" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="286" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A286">
+        <v>844</v>
+      </c>
+      <c r="B286">
+        <v>284</v>
+      </c>
+      <c r="C286">
+        <v>11</v>
+      </c>
+      <c r="D286">
+        <v>2</v>
+      </c>
+      <c r="E286" t="s">
+        <v>885</v>
+      </c>
+      <c r="F286" t="s">
+        <v>865</v>
+      </c>
+      <c r="G286">
+        <v>6</v>
+      </c>
+      <c r="I286">
+        <v>0</v>
+      </c>
+      <c r="J286" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="287" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A287">
+        <v>847</v>
+      </c>
+      <c r="B287">
+        <v>285</v>
+      </c>
+      <c r="C287">
+        <v>11</v>
+      </c>
+      <c r="D287">
+        <v>2</v>
+      </c>
+      <c r="E287" t="s">
+        <v>885</v>
+      </c>
+      <c r="F287" t="s">
+        <v>865</v>
+      </c>
+      <c r="G287">
+        <v>10</v>
+      </c>
+      <c r="I287">
+        <v>0</v>
+      </c>
+      <c r="J287" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="288" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A288">
+        <v>849</v>
+      </c>
+      <c r="B288">
+        <v>286</v>
+      </c>
+      <c r="C288">
+        <v>11</v>
+      </c>
+      <c r="D288">
+        <v>2</v>
+      </c>
+      <c r="E288" t="s">
+        <v>885</v>
+      </c>
+      <c r="F288" t="s">
+        <v>865</v>
+      </c>
+      <c r="G288">
+        <v>14</v>
+      </c>
+      <c r="I288">
+        <v>0</v>
+      </c>
+      <c r="J288" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="289" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A289">
+        <v>853</v>
+      </c>
+      <c r="B289">
+        <v>287</v>
+      </c>
+      <c r="C289">
+        <v>12</v>
+      </c>
+      <c r="D289">
+        <v>1</v>
+      </c>
+      <c r="E289" t="s">
+        <v>849</v>
+      </c>
+      <c r="I289">
+        <v>0</v>
+      </c>
+      <c r="J289" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="290" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A290">
+        <v>855</v>
+      </c>
+      <c r="B290">
+        <v>288</v>
+      </c>
+      <c r="C290">
+        <v>12</v>
+      </c>
+      <c r="D290">
+        <v>2</v>
+      </c>
+      <c r="E290" t="s">
+        <v>849</v>
+      </c>
+      <c r="F290" t="s">
+        <v>863</v>
+      </c>
+      <c r="G290">
+        <v>1</v>
+      </c>
+      <c r="I290">
+        <v>0</v>
+      </c>
+      <c r="J290" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="291" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A291">
+        <v>857</v>
+      </c>
+      <c r="B291">
+        <v>289</v>
+      </c>
+      <c r="C291">
+        <v>12</v>
+      </c>
+      <c r="D291">
+        <v>2</v>
+      </c>
+      <c r="E291" t="s">
+        <v>849</v>
+      </c>
+      <c r="F291" t="s">
+        <v>863</v>
+      </c>
+      <c r="G291">
+        <v>1</v>
+      </c>
+      <c r="I291">
+        <v>0</v>
+      </c>
+      <c r="J291" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="292" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A292">
+        <v>867</v>
+      </c>
+      <c r="B292">
+        <v>290</v>
+      </c>
+      <c r="C292">
+        <v>12</v>
+      </c>
+      <c r="D292">
+        <v>2</v>
+      </c>
+      <c r="E292" t="s">
+        <v>849</v>
+      </c>
+      <c r="F292" t="s">
+        <v>863</v>
+      </c>
+      <c r="G292">
+        <v>1</v>
+      </c>
+      <c r="I292">
+        <v>0</v>
+      </c>
+      <c r="J292" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="293" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A293">
+        <v>872</v>
+      </c>
+      <c r="B293">
+        <v>291</v>
+      </c>
+      <c r="C293">
+        <v>12</v>
+      </c>
+      <c r="D293">
+        <v>2</v>
+      </c>
+      <c r="E293" t="s">
+        <v>849</v>
+      </c>
+      <c r="F293" t="s">
+        <v>863</v>
+      </c>
+      <c r="G293">
+        <v>1</v>
+      </c>
+      <c r="I293">
+        <v>0</v>
+      </c>
+      <c r="J293" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="294" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A294">
+        <v>876</v>
+      </c>
+      <c r="B294">
+        <v>292</v>
+      </c>
+      <c r="C294">
+        <v>12</v>
+      </c>
+      <c r="D294">
+        <v>2</v>
+      </c>
+      <c r="E294" t="s">
+        <v>849</v>
+      </c>
+      <c r="F294" t="s">
+        <v>863</v>
+      </c>
+      <c r="G294">
+        <v>1</v>
+      </c>
+      <c r="I294">
+        <v>0</v>
+      </c>
+      <c r="J294" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="295" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A295">
+        <v>878</v>
+      </c>
+      <c r="B295">
+        <v>293</v>
+      </c>
+      <c r="C295">
+        <v>12</v>
+      </c>
+      <c r="D295">
+        <v>2</v>
+      </c>
+      <c r="E295" t="s">
+        <v>849</v>
+      </c>
+      <c r="F295" t="s">
+        <v>863</v>
+      </c>
+      <c r="G295">
+        <v>1</v>
+      </c>
+      <c r="I295">
+        <v>0</v>
+      </c>
+      <c r="J295" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="296" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A296">
+        <v>880</v>
+      </c>
+      <c r="B296">
+        <v>294</v>
+      </c>
+      <c r="C296">
+        <v>12</v>
+      </c>
+      <c r="D296">
+        <v>2</v>
+      </c>
+      <c r="E296" t="s">
+        <v>849</v>
+      </c>
+      <c r="F296" t="s">
+        <v>863</v>
+      </c>
+      <c r="G296">
+        <v>1</v>
+      </c>
+      <c r="I296">
+        <v>0</v>
+      </c>
+      <c r="J296" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="297" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A297">
+        <v>882</v>
+      </c>
+      <c r="B297">
+        <v>295</v>
+      </c>
+      <c r="C297">
+        <v>12</v>
+      </c>
+      <c r="D297">
+        <v>1</v>
+      </c>
+      <c r="E297" t="s">
+        <v>849</v>
+      </c>
+      <c r="F297" t="s">
+        <v>863</v>
+      </c>
+      <c r="G297">
+        <v>1</v>
+      </c>
+      <c r="I297">
+        <v>0</v>
+      </c>
+      <c r="J297" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="298" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A298">
+        <v>885</v>
+      </c>
+      <c r="B298">
+        <v>296</v>
+      </c>
+      <c r="C298">
+        <v>12</v>
+      </c>
+      <c r="D298">
+        <v>1</v>
+      </c>
+      <c r="E298" t="s">
+        <v>849</v>
+      </c>
+      <c r="F298" t="s">
+        <v>863</v>
+      </c>
+      <c r="G298">
+        <v>2</v>
+      </c>
+      <c r="I298">
+        <v>0</v>
+      </c>
+      <c r="J298" t="s">
+        <v>800</v>
+      </c>
+      <c r="K298" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="299" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A299">
+        <v>888</v>
+      </c>
+      <c r="B299">
+        <v>297</v>
+      </c>
+      <c r="C299">
+        <v>12</v>
+      </c>
+      <c r="D299">
+        <v>1</v>
+      </c>
+      <c r="E299" t="s">
+        <v>849</v>
+      </c>
+      <c r="F299" t="s">
+        <v>864</v>
+      </c>
+      <c r="G299">
+        <v>4</v>
+      </c>
+      <c r="I299">
+        <v>0</v>
+      </c>
+      <c r="J299" t="s">
+        <v>66</v>
+      </c>
+      <c r="K299" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="300" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A300">
+        <v>890</v>
+      </c>
+      <c r="B300">
+        <v>298</v>
+      </c>
+      <c r="C300">
+        <v>12</v>
+      </c>
+      <c r="D300">
+        <v>1</v>
+      </c>
+      <c r="E300" t="s">
+        <v>849</v>
+      </c>
+      <c r="F300" t="s">
+        <v>863</v>
+      </c>
+      <c r="G300">
+        <v>18</v>
+      </c>
+      <c r="I300">
+        <v>0</v>
+      </c>
+      <c r="J300" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="301" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A301">
+        <v>893</v>
+      </c>
+      <c r="B301">
+        <v>299</v>
+      </c>
+      <c r="E301" t="s">
+        <v>849</v>
+      </c>
+      <c r="F301" t="s">
+        <v>863</v>
+      </c>
+      <c r="G301">
+        <v>20</v>
+      </c>
+      <c r="J301" t="s">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="302" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A302">
+        <v>895</v>
+      </c>
+      <c r="B302">
+        <v>300</v>
+      </c>
+      <c r="C302">
+        <v>12</v>
+      </c>
+      <c r="D302">
+        <v>1</v>
+      </c>
+      <c r="E302" t="s">
+        <v>807</v>
+      </c>
+      <c r="F302" t="s">
+        <v>865</v>
+      </c>
+      <c r="G302">
+        <v>2</v>
+      </c>
+      <c r="I302">
+        <v>0</v>
+      </c>
+      <c r="J302" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="303" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A303">
+        <v>897</v>
+      </c>
+      <c r="B303">
+        <v>301</v>
+      </c>
+      <c r="C303">
+        <v>12</v>
+      </c>
+      <c r="D303">
+        <v>2</v>
+      </c>
+      <c r="E303" t="s">
+        <v>807</v>
+      </c>
+      <c r="F303" t="s">
+        <v>865</v>
+      </c>
+      <c r="G303">
+        <v>2</v>
+      </c>
+      <c r="I303">
+        <v>0</v>
+      </c>
+      <c r="J303" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="304" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A304">
+        <v>899</v>
+      </c>
+      <c r="B304">
+        <v>302</v>
+      </c>
+      <c r="C304">
+        <v>12</v>
+      </c>
+      <c r="D304">
+        <v>2</v>
+      </c>
+      <c r="E304" t="s">
+        <v>807</v>
+      </c>
+      <c r="F304" t="s">
+        <v>865</v>
+      </c>
+      <c r="G304">
+        <v>2</v>
+      </c>
+      <c r="I304">
+        <v>0</v>
+      </c>
+      <c r="J304" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="305" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A305">
+        <v>901</v>
+      </c>
+      <c r="B305">
+        <v>303</v>
+      </c>
+      <c r="C305">
+        <v>12</v>
+      </c>
+      <c r="D305">
+        <v>2</v>
+      </c>
+      <c r="E305" t="s">
+        <v>807</v>
+      </c>
+      <c r="F305" t="s">
+        <v>865</v>
+      </c>
+      <c r="G305">
+        <v>6</v>
+      </c>
+      <c r="I305">
+        <v>0</v>
+      </c>
+      <c r="J305" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="306" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A306">
+        <v>903</v>
+      </c>
+      <c r="B306">
+        <v>304</v>
+      </c>
+      <c r="C306">
+        <v>12</v>
+      </c>
+      <c r="D306">
+        <v>2</v>
+      </c>
+      <c r="E306" t="s">
+        <v>807</v>
+      </c>
+      <c r="F306" t="s">
+        <v>865</v>
+      </c>
+      <c r="G306">
+        <v>10</v>
+      </c>
+      <c r="I306">
+        <v>0</v>
+      </c>
+      <c r="J306" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="307" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A307">
+        <v>905</v>
+      </c>
+      <c r="B307">
+        <v>305</v>
+      </c>
+      <c r="C307">
+        <v>12</v>
+      </c>
+      <c r="D307">
+        <v>2</v>
+      </c>
+      <c r="E307" t="s">
+        <v>807</v>
+      </c>
+      <c r="F307" t="s">
+        <v>865</v>
+      </c>
+      <c r="G307">
+        <v>14</v>
+      </c>
+      <c r="I307">
+        <v>0</v>
+      </c>
+      <c r="J307" t="s">
+        <v>817</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Jun 18, 2024, 3:16 PM
</commit_message>
<xml_diff>
--- a/Main/static/CSVs/Features List.xlsx
+++ b/Main/static/CSVs/Features List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitProjects\CS50-FinalProject\Main\static\CSVs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7741A1C4-E07D-4CFE-8145-3CD60D673A9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF5C1A5-B791-4FB8-8CEC-9CF1E1BF89D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="features_list" sheetId="3" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3183" uniqueCount="880">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3184" uniqueCount="881">
   <si>
     <t>Metadata:</t>
   </si>
@@ -2671,6 +2671,9 @@
   </si>
   <si>
     <t>NOTES:</t>
+  </si>
+  <si>
+    <t>figh</t>
   </si>
 </sst>
 </file>
@@ -2777,7 +2780,14 @@
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{581F8D43-91C3-4934-AAB2-DF443FB59E02}" name="Table2" displayName="Table2" ref="A1:J307" totalsRowShown="0">
-  <autoFilter ref="A1:J307" xr:uid="{581F8D43-91C3-4934-AAB2-DF443FB59E02}"/>
+  <autoFilter ref="A1:J307" xr:uid="{581F8D43-91C3-4934-AAB2-DF443FB59E02}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="5"/>
+        <filter val="12"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="10">
     <tableColumn id="11" xr3:uid="{7F2D1C90-1015-492A-99DD-277581E9724D}" name=" feature_id"/>
     <tableColumn id="2" xr3:uid="{C50FB54B-3D91-4D5B-8972-3D51810DA21B}" name=" feature_from_class"/>
@@ -3059,8 +3069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1000DAD0-45D8-4F57-BB32-ED68B84F1CCC}">
   <dimension ref="A1:F910"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D296" sqref="D296"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D187" sqref="D187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21284,10 +21294,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF617F07-646C-48AF-866C-AB0475963108}">
-  <dimension ref="A1:L307"/>
+  <dimension ref="A1:M307"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21304,7 +21314,7 @@
     <col min="12" max="12" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>35</v>
       </c>
@@ -21339,7 +21349,7 @@
         <v>879</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -21365,7 +21375,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -21394,7 +21404,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -21423,7 +21433,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -21452,7 +21462,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -21480,8 +21490,11 @@
       <c r="J6" t="s">
         <v>852</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M6" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -21513,7 +21526,7 @@
         <v>859</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -21542,7 +21555,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -21571,7 +21584,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -21600,7 +21613,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -21632,7 +21645,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -21661,7 +21674,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -21690,7 +21703,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -21719,7 +21732,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -21745,7 +21758,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -21774,7 +21787,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -21803,7 +21816,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -21832,7 +21845,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -21861,7 +21874,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -21890,7 +21903,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -21916,7 +21929,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
@@ -21945,7 +21958,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
@@ -21974,7 +21987,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
@@ -22003,7 +22016,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
@@ -22032,7 +22045,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
@@ -22061,7 +22074,7 @@
         <v>871</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
@@ -22090,7 +22103,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
@@ -22119,7 +22132,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
@@ -22151,7 +22164,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
@@ -22183,7 +22196,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
@@ -22215,7 +22228,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
@@ -22247,7 +22260,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
@@ -22273,7 +22286,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
@@ -22302,7 +22315,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
@@ -22334,7 +22347,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>34</v>
       </c>
@@ -22363,7 +22376,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
@@ -22389,7 +22402,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
@@ -22418,7 +22431,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
@@ -22447,7 +22460,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>38</v>
       </c>
@@ -22476,7 +22489,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>39</v>
       </c>
@@ -22502,7 +22515,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>40</v>
       </c>
@@ -22534,7 +22547,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>41</v>
       </c>
@@ -22563,7 +22576,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>42</v>
       </c>
@@ -22592,7 +22605,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>43</v>
       </c>
@@ -22618,7 +22631,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>44</v>
       </c>
@@ -22644,7 +22657,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>45</v>
       </c>
@@ -22670,7 +22683,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>46</v>
       </c>
@@ -22699,7 +22712,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>47</v>
       </c>
@@ -22728,7 +22741,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>48</v>
       </c>
@@ -22757,7 +22770,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>49</v>
       </c>
@@ -22783,7 +22796,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>50</v>
       </c>
@@ -22812,7 +22825,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>51</v>
       </c>
@@ -22841,7 +22854,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>52</v>
       </c>
@@ -22870,7 +22883,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>53</v>
       </c>
@@ -22896,7 +22909,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>54</v>
       </c>
@@ -22922,7 +22935,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>55</v>
       </c>
@@ -22948,7 +22961,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>56</v>
       </c>
@@ -22974,7 +22987,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>57</v>
       </c>
@@ -23000,7 +23013,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>58</v>
       </c>
@@ -23026,7 +23039,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>59</v>
       </c>
@@ -23052,7 +23065,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>60</v>
       </c>
@@ -23078,7 +23091,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>61</v>
       </c>
@@ -23107,7 +23120,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>62</v>
       </c>
@@ -23136,7 +23149,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>63</v>
       </c>
@@ -23165,7 +23178,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>64</v>
       </c>
@@ -23191,7 +23204,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>65</v>
       </c>
@@ -23217,7 +23230,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>66</v>
       </c>
@@ -23243,7 +23256,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>67</v>
       </c>
@@ -23272,7 +23285,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>68</v>
       </c>
@@ -23301,7 +23314,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>69</v>
       </c>
@@ -23330,7 +23343,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>70</v>
       </c>
@@ -23356,7 +23369,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>71</v>
       </c>
@@ -23382,7 +23395,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>72</v>
       </c>
@@ -23408,7 +23421,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>73</v>
       </c>
@@ -23434,7 +23447,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>74</v>
       </c>
@@ -23460,7 +23473,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>75</v>
       </c>
@@ -23486,7 +23499,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>76</v>
       </c>
@@ -23515,7 +23528,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>77</v>
       </c>
@@ -23541,7 +23554,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>78</v>
       </c>
@@ -23567,7 +23580,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>79</v>
       </c>
@@ -24102,7 +24115,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>99</v>
       </c>
@@ -24128,7 +24141,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>100</v>
       </c>
@@ -24154,7 +24167,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>101</v>
       </c>
@@ -24183,7 +24196,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>102</v>
       </c>
@@ -24209,7 +24222,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>103</v>
       </c>
@@ -24235,7 +24248,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>104</v>
       </c>
@@ -24261,7 +24274,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>105</v>
       </c>
@@ -24287,7 +24300,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>106</v>
       </c>
@@ -24313,7 +24326,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>107</v>
       </c>
@@ -24339,7 +24352,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>108</v>
       </c>
@@ -24368,7 +24381,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>109</v>
       </c>
@@ -24394,7 +24407,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>110</v>
       </c>
@@ -24420,7 +24433,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>111</v>
       </c>
@@ -24446,7 +24459,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>112</v>
       </c>
@@ -24472,7 +24485,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>113</v>
       </c>
@@ -24498,7 +24511,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>114</v>
       </c>
@@ -24524,7 +24537,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>115</v>
       </c>
@@ -24550,7 +24563,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>116</v>
       </c>
@@ -24576,7 +24589,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>117</v>
       </c>
@@ -24602,7 +24615,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>118</v>
       </c>
@@ -24628,7 +24641,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>119</v>
       </c>
@@ -24654,7 +24667,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>120</v>
       </c>
@@ -24680,7 +24693,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>121</v>
       </c>
@@ -24706,7 +24719,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>122</v>
       </c>
@@ -24732,7 +24745,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>123</v>
       </c>
@@ -24758,7 +24771,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>124</v>
       </c>
@@ -24784,7 +24797,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>125</v>
       </c>
@@ -24810,7 +24823,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>126</v>
       </c>
@@ -24836,7 +24849,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>127</v>
       </c>
@@ -24862,7 +24875,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>128</v>
       </c>
@@ -24888,7 +24901,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>129</v>
       </c>
@@ -24914,7 +24927,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>130</v>
       </c>
@@ -24940,7 +24953,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>131</v>
       </c>
@@ -24966,7 +24979,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>132</v>
       </c>
@@ -24992,7 +25005,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>133</v>
       </c>
@@ -25018,7 +25031,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>134</v>
       </c>
@@ -25044,7 +25057,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>135</v>
       </c>
@@ -25070,7 +25083,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>136</v>
       </c>
@@ -25096,7 +25109,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>137</v>
       </c>
@@ -25122,7 +25135,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>138</v>
       </c>
@@ -25148,7 +25161,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>139</v>
       </c>
@@ -25174,7 +25187,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>140</v>
       </c>
@@ -25203,7 +25216,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>141</v>
       </c>
@@ -25232,7 +25245,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>142</v>
       </c>
@@ -25261,7 +25274,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>143</v>
       </c>
@@ -25290,7 +25303,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>144</v>
       </c>
@@ -25316,7 +25329,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>145</v>
       </c>
@@ -25345,7 +25358,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>146</v>
       </c>
@@ -25374,7 +25387,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>147</v>
       </c>
@@ -25400,7 +25413,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>148</v>
       </c>
@@ -25426,7 +25439,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>149</v>
       </c>
@@ -25452,7 +25465,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>150</v>
       </c>
@@ -25478,7 +25491,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>151</v>
       </c>
@@ -25507,7 +25520,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>152</v>
       </c>
@@ -25533,7 +25546,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>153</v>
       </c>
@@ -25559,7 +25572,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>154</v>
       </c>
@@ -25585,7 +25598,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>155</v>
       </c>
@@ -25611,7 +25624,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>156</v>
       </c>
@@ -25637,7 +25650,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>157</v>
       </c>
@@ -25663,7 +25676,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>158</v>
       </c>
@@ -25689,7 +25702,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>159</v>
       </c>
@@ -25715,7 +25728,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>160</v>
       </c>
@@ -25741,7 +25754,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>161</v>
       </c>
@@ -25767,7 +25780,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>162</v>
       </c>
@@ -25793,7 +25806,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>163</v>
       </c>
@@ -25819,7 +25832,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>164</v>
       </c>
@@ -25845,7 +25858,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>165</v>
       </c>
@@ -25871,7 +25884,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>166</v>
       </c>
@@ -25897,7 +25910,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>167</v>
       </c>
@@ -25923,7 +25936,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>168</v>
       </c>
@@ -25949,7 +25962,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>169</v>
       </c>
@@ -25978,7 +25991,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>170</v>
       </c>
@@ -26007,7 +26020,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>171</v>
       </c>
@@ -26036,7 +26049,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>172</v>
       </c>
@@ -26062,7 +26075,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>173</v>
       </c>
@@ -26088,7 +26101,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>174</v>
       </c>
@@ -26114,7 +26127,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>175</v>
       </c>
@@ -26140,7 +26153,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="178" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>176</v>
       </c>
@@ -26166,7 +26179,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="179" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>177</v>
       </c>
@@ -26192,7 +26205,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>178</v>
       </c>
@@ -26218,7 +26231,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="181" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>179</v>
       </c>
@@ -26244,7 +26257,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="182" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>180</v>
       </c>
@@ -26270,7 +26283,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="183" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>181</v>
       </c>
@@ -26296,7 +26309,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="184" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>182</v>
       </c>
@@ -26322,7 +26335,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="185" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>183</v>
       </c>
@@ -26348,7 +26361,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="186" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>184</v>
       </c>
@@ -26374,7 +26387,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>185</v>
       </c>
@@ -26403,7 +26416,7 @@
         <v>872</v>
       </c>
     </row>
-    <row r="188" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>186</v>
       </c>
@@ -26429,7 +26442,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="189" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>187</v>
       </c>
@@ -26455,7 +26468,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="190" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>188</v>
       </c>
@@ -26481,7 +26494,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="191" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>189</v>
       </c>
@@ -26507,7 +26520,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="192" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>190</v>
       </c>
@@ -26533,7 +26546,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>191</v>
       </c>
@@ -26559,7 +26572,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>192</v>
       </c>
@@ -26585,7 +26598,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>193</v>
       </c>
@@ -26611,7 +26624,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>194</v>
       </c>
@@ -26637,7 +26650,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>195</v>
       </c>
@@ -26663,7 +26676,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>196</v>
       </c>
@@ -26689,7 +26702,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>197</v>
       </c>
@@ -26715,7 +26728,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>198</v>
       </c>
@@ -26741,7 +26754,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>199</v>
       </c>
@@ -26764,7 +26777,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>200</v>
       </c>
@@ -26790,7 +26803,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>201</v>
       </c>
@@ -26816,7 +26829,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>202</v>
       </c>
@@ -26842,7 +26855,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>203</v>
       </c>
@@ -26868,7 +26881,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>204</v>
       </c>
@@ -26894,7 +26907,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>205</v>
       </c>
@@ -26920,7 +26933,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>206</v>
       </c>
@@ -26946,7 +26959,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>207</v>
       </c>
@@ -26972,7 +26985,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>208</v>
       </c>
@@ -26998,7 +27011,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>209</v>
       </c>
@@ -27024,7 +27037,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>210</v>
       </c>
@@ -27050,7 +27063,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>211</v>
       </c>
@@ -27076,7 +27089,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>212</v>
       </c>
@@ -27105,7 +27118,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>213</v>
       </c>
@@ -27131,7 +27144,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>214</v>
       </c>
@@ -27160,7 +27173,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>215</v>
       </c>
@@ -27189,7 +27202,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>216</v>
       </c>
@@ -27215,7 +27228,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>217</v>
       </c>
@@ -27241,7 +27254,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>218</v>
       </c>
@@ -27267,7 +27280,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>219</v>
       </c>
@@ -27293,7 +27306,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>220</v>
       </c>
@@ -27319,7 +27332,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>221</v>
       </c>
@@ -27345,7 +27358,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>222</v>
       </c>
@@ -27371,7 +27384,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>223</v>
       </c>
@@ -27397,7 +27410,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>224</v>
       </c>
@@ -27423,7 +27436,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>225</v>
       </c>
@@ -27452,7 +27465,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>226</v>
       </c>
@@ -27475,7 +27488,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>227</v>
       </c>
@@ -27501,7 +27514,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>228</v>
       </c>
@@ -27527,7 +27540,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>229</v>
       </c>
@@ -27553,7 +27566,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>230</v>
       </c>
@@ -27579,7 +27592,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>231</v>
       </c>
@@ -27605,7 +27618,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>232</v>
       </c>
@@ -27634,7 +27647,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>233</v>
       </c>
@@ -27663,7 +27676,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>234</v>
       </c>
@@ -27689,7 +27702,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>235</v>
       </c>
@@ -27715,7 +27728,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>236</v>
       </c>
@@ -27741,7 +27754,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>237</v>
       </c>
@@ -27767,7 +27780,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>238</v>
       </c>
@@ -27793,7 +27806,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>239</v>
       </c>
@@ -27819,7 +27832,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>240</v>
       </c>
@@ -27848,7 +27861,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>241</v>
       </c>
@@ -27877,7 +27890,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>242</v>
       </c>
@@ -27903,7 +27916,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>243</v>
       </c>
@@ -27929,7 +27942,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>244</v>
       </c>
@@ -27955,7 +27968,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>245</v>
       </c>
@@ -27984,7 +27997,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>246</v>
       </c>
@@ -28013,7 +28026,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>247</v>
       </c>
@@ -28039,7 +28052,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>248</v>
       </c>
@@ -28062,7 +28075,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>249</v>
       </c>
@@ -28088,7 +28101,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252">
         <v>250</v>
       </c>
@@ -28114,7 +28127,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>251</v>
       </c>
@@ -28140,7 +28153,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A254">
         <v>252</v>
       </c>
@@ -28166,7 +28179,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A255">
         <v>253</v>
       </c>
@@ -28192,7 +28205,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A256">
         <v>254</v>
       </c>
@@ -28218,7 +28231,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="257" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A257">
         <v>255</v>
       </c>
@@ -28244,7 +28257,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="258" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A258">
         <v>256</v>
       </c>
@@ -28270,7 +28283,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="259" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259">
         <v>257</v>
       </c>
@@ -28296,7 +28309,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="260" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A260">
         <v>258</v>
       </c>
@@ -28322,7 +28335,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="261" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A261">
         <v>259</v>
       </c>
@@ -28348,7 +28361,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="262" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A262">
         <v>260</v>
       </c>
@@ -28374,7 +28387,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="263" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A263">
         <v>261</v>
       </c>
@@ -28400,7 +28413,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="264" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A264">
         <v>262</v>
       </c>
@@ -28426,7 +28439,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="265" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A265">
         <v>263</v>
       </c>
@@ -28452,7 +28465,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="266" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266">
         <v>264</v>
       </c>
@@ -28478,7 +28491,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="267" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267">
         <v>265</v>
       </c>
@@ -28504,7 +28517,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="268" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A268">
         <v>266</v>
       </c>
@@ -28530,7 +28543,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="269" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A269">
         <v>267</v>
       </c>
@@ -28556,7 +28569,7 @@
         <v>875</v>
       </c>
     </row>
-    <row r="270" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A270">
         <v>268</v>
       </c>
@@ -28582,7 +28595,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="271" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A271">
         <v>269</v>
       </c>
@@ -28608,7 +28621,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="272" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A272">
         <v>270</v>
       </c>
@@ -28634,7 +28647,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="273" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A273">
         <v>271</v>
       </c>
@@ -28660,7 +28673,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="274" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A274">
         <v>272</v>
       </c>
@@ -28686,7 +28699,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="275" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A275">
         <v>273</v>
       </c>
@@ -28712,7 +28725,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="276" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A276">
         <v>274</v>
       </c>
@@ -28738,7 +28751,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="277" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A277">
         <v>275</v>
       </c>
@@ -28764,7 +28777,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="278" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A278">
         <v>276</v>
       </c>
@@ -28790,7 +28803,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="279" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A279">
         <v>277</v>
       </c>
@@ -28816,7 +28829,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="280" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A280">
         <v>278</v>
       </c>
@@ -28842,7 +28855,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="281" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A281">
         <v>279</v>
       </c>
@@ -28868,7 +28881,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="282" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A282">
         <v>280</v>
       </c>
@@ -28894,7 +28907,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="283" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A283">
         <v>281</v>
       </c>
@@ -28923,7 +28936,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="284" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A284">
         <v>282</v>
       </c>
@@ -28949,7 +28962,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="285" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A285">
         <v>283</v>
       </c>
@@ -28975,7 +28988,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="286" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A286">
         <v>284</v>
       </c>
@@ -29001,7 +29014,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="287" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A287">
         <v>285</v>
       </c>
@@ -29027,7 +29040,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="288" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A288">
         <v>286</v>
       </c>
@@ -29549,8 +29562,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -37750,7 +37764,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:I26"/>
+      <selection activeCell="A18" sqref="A12:A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37899,7 +37913,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9C2A960-F8A0-4080-979F-D89E63FD0EF6}">
   <dimension ref="A1:F99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>

<commit_message>
Jun 23, 2024, 2:11 PM
</commit_message>
<xml_diff>
--- a/Main/static/CSVs/Features List.xlsx
+++ b/Main/static/CSVs/Features List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitProjects\CS50-FinalProject\Main\static\CSVs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE6689C3-F595-454B-990D-0DF44B2A3607}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9845A40C-1590-4B21-BE25-8D4B62E0CA5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3055,7 +3055,7 @@
   <dimension ref="A1:F909"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C293" sqref="C293"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8939,7 +8939,7 @@
         <v>4</v>
       </c>
       <c r="D294">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E294">
         <v>0</v>
@@ -21262,7 +21262,7 @@
   <dimension ref="A1:L307"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="M46" sqref="M46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23758,7 +23758,7 @@
         <v>4</v>
       </c>
       <c r="C89">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D89">
         <v>0</v>
@@ -29725,7 +29725,7 @@
   <dimension ref="A1:F98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30041,7 +30041,7 @@
         <v>4</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E16">
         <v>0</v>

</xml_diff>